<commit_message>
updating for changes to wc-lang author.orcid, DatabaseReference-->Identifier
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/2_species_1_reaction_with_rates_given_by_reactant_population.xlsx
+++ b/tests/multialgorithm/fixtures/2_species_1_reaction_with_rates_given_by_reactant_population.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="993" firstSheet="7" activeTab="18"/>
+    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="993" firstSheet="13" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="24" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="160">
   <si>
     <t>Table</t>
   </si>
@@ -216,7 +216,7 @@
     <t>s</t>
   </si>
   <si>
-    <t>Database references</t>
+    <t>Identifiers</t>
   </si>
   <si>
     <t>Comments</t>
@@ -558,9 +558,6 @@
     <t>Address</t>
   </si>
   <si>
-    <t>ORCID</t>
-  </si>
-  <si>
     <t>Target</t>
   </si>
   <si>
@@ -590,10 +587,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -647,6 +644,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -655,28 +667,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -698,9 +691,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -714,24 +734,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -744,9 +748,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -767,30 +786,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -817,7 +814,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -829,7 +826,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,103 +982,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -949,55 +994,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1011,11 +1008,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1024,7 +1042,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1045,21 +1063,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1074,17 +1077,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1111,138 +1108,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2675,12 +2672,12 @@
   <sheetPr/>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1:V2"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
@@ -3077,14 +3074,14 @@
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K$1:K$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -3092,7 +3089,7 @@
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:13">
+    <row r="1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -3124,12 +3121,9 @@
         <v>151</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3168,25 +3162,25 @@
         <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>38</v>
@@ -3207,7 +3201,7 @@
         <v>23</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>